<commit_message>
Submitted the design for manufacturing
</commit_message>
<xml_diff>
--- a/2sets-BOM.xlsx
+++ b/2sets-BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashahs\source\repos\PCBChamberRTDs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amirs\repos\PCBChamberRTDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57A56E1-0518-476D-8B0D-9B32C7999761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE546DA-CFE0-440B-8D88-D860940D178C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1078,9 +1078,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1095,6 +1092,9 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1477,26 +1477,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ974"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
     <col min="6" max="6" width="27" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="103"/>
-    <col min="14" max="14" width="14.42578125" style="104"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" customWidth="1"/>
+    <col min="11" max="11" width="4.44140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="103"/>
+    <col min="14" max="14" width="14.44140625" style="104"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="12.75" customHeight="1">
@@ -1583,10 +1583,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="16"/>
-      <c r="G7" s="123">
+      <c r="G7" s="128">
         <v>44571</v>
       </c>
-      <c r="H7" s="123"/>
+      <c r="H7" s="128"/>
       <c r="I7" s="67"/>
       <c r="J7" s="58"/>
       <c r="K7" s="59"/>
@@ -1598,8 +1598,8 @@
         <v>24</v>
       </c>
       <c r="F8" s="18"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
       <c r="I8" s="67"/>
       <c r="J8" s="58"/>
       <c r="K8" s="59"/>
@@ -1750,10 +1750,10 @@
       <c r="D13" s="25">
         <v>2</v>
       </c>
-      <c r="E13" s="125" t="s">
+      <c r="E13" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="126" t="s">
+      <c r="F13" s="125" t="s">
         <v>58</v>
       </c>
       <c r="G13" s="72" t="s">
@@ -1863,7 +1863,7 @@
       <c r="E15" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="126" t="s">
+      <c r="F15" s="125" t="s">
         <v>78</v>
       </c>
       <c r="G15" s="72" t="s">
@@ -2022,13 +2022,13 @@
     <row r="18" spans="1:36" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="123" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="25">
         <v>6</v>
       </c>
-      <c r="E18" s="125" t="s">
+      <c r="E18" s="124" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="27" t="s">
@@ -2080,11 +2080,11 @@
     <row r="19" spans="1:36" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
-      <c r="C19" s="124"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="25">
         <v>7</v>
       </c>
-      <c r="E19" s="125" t="s">
+      <c r="E19" s="124" t="s">
         <v>83</v>
       </c>
       <c r="F19" s="27" t="s">
@@ -2138,7 +2138,7 @@
       <c r="D20" s="25">
         <v>8</v>
       </c>
-      <c r="E20" s="125" t="s">
+      <c r="E20" s="124" t="s">
         <v>67</v>
       </c>
       <c r="F20" s="27" t="s">
@@ -2296,7 +2296,7 @@
       <c r="D23" s="25">
         <v>11</v>
       </c>
-      <c r="E23" s="127" t="s">
+      <c r="E23" s="126" t="s">
         <v>76</v>
       </c>
       <c r="F23" s="112" t="s">
@@ -2402,7 +2402,7 @@
       <c r="D25" s="25">
         <v>13</v>
       </c>
-      <c r="E25" s="128" t="s">
+      <c r="E25" s="127" t="s">
         <v>86</v>
       </c>
       <c r="F25" s="29">
@@ -2447,7 +2447,7 @@
       <c r="AI25"/>
       <c r="AJ25"/>
     </row>
-    <row r="26" spans="1:36" s="2" customFormat="1" ht="28.9" customHeight="1">
+    <row r="26" spans="1:36" s="2" customFormat="1" ht="28.95" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="24"/>
       <c r="C26" s="20"/>
@@ -2485,7 +2485,7 @@
       <c r="AI26"/>
       <c r="AJ26"/>
     </row>
-    <row r="27" spans="1:36" ht="42.95" customHeight="1">
+    <row r="27" spans="1:36" ht="42.9" customHeight="1">
       <c r="A27" s="100" t="s">
         <v>19</v>
       </c>

</xml_diff>